<commit_message>
update apjc addressable tracker
</commit_message>
<xml_diff>
--- a/tracker/apjc_history_addressable.xlsx
+++ b/tracker/apjc_history_addressable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangken/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangken/py/dfpm_tools/tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B3169E-7172-364A-B96D-FAEF75D1F2EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5DA0054-9E80-774A-93D8-B264D6745930}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APJC" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2077" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2161" uniqueCount="389">
   <si>
     <t>APJC</t>
   </si>
@@ -1065,6 +1065,42 @@
     <t>2021-02-24</t>
   </si>
   <si>
+    <t>2021-02-25</t>
+  </si>
+  <si>
+    <t>2021-02-26</t>
+  </si>
+  <si>
+    <t>2021-03-01</t>
+  </si>
+  <si>
+    <t>2021-03-02</t>
+  </si>
+  <si>
+    <t>2021-03-03</t>
+  </si>
+  <si>
+    <t>2021-03-04</t>
+  </si>
+  <si>
+    <t>2021-03-05</t>
+  </si>
+  <si>
+    <t>2021-03-08</t>
+  </si>
+  <si>
+    <t>2021-03-10</t>
+  </si>
+  <si>
+    <t>2021-03-11</t>
+  </si>
+  <si>
+    <t>2021-03-12</t>
+  </si>
+  <si>
+    <t>2021-03-15</t>
+  </si>
+  <si>
     <t>ERBU</t>
   </si>
   <si>
@@ -1090,9 +1126,6 @@
   </si>
   <si>
     <t>INSBU</t>
-  </si>
-  <si>
-    <t>CRBU-other</t>
   </si>
   <si>
     <t>EBBU</t>
@@ -1134,6 +1167,9 @@
     <t>ONPREMCONTCENTERBU</t>
   </si>
   <si>
+    <t>CRBU-other</t>
+  </si>
+  <si>
     <t>TMGBU</t>
   </si>
   <si>
@@ -1156,9 +1192,6 @@
   </si>
   <si>
     <t>OTBU</t>
-  </si>
-  <si>
-    <t>CRBU-OTHER</t>
   </si>
 </sst>
 </file>
@@ -1560,7 +1593,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H381"/>
+  <dimension ref="A1:H395"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10545,6 +10578,328 @@
         <v>16.5</v>
       </c>
     </row>
+    <row r="382" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A382" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B382">
+        <v>979.5</v>
+      </c>
+      <c r="C382">
+        <v>485.2</v>
+      </c>
+      <c r="D382">
+        <v>74.8</v>
+      </c>
+      <c r="E382">
+        <v>34.1</v>
+      </c>
+      <c r="F382">
+        <v>369.3</v>
+      </c>
+      <c r="H382">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="383" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A383" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B383">
+        <v>994</v>
+      </c>
+      <c r="C383">
+        <v>497.4</v>
+      </c>
+      <c r="D383">
+        <v>75.8</v>
+      </c>
+      <c r="E383">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="F383">
+        <v>368.8</v>
+      </c>
+      <c r="H383">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="384" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A384" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B384">
+        <v>994.5</v>
+      </c>
+      <c r="C384">
+        <v>501.5</v>
+      </c>
+      <c r="D384">
+        <v>78</v>
+      </c>
+      <c r="E384">
+        <v>33.9</v>
+      </c>
+      <c r="F384">
+        <v>365.1</v>
+      </c>
+      <c r="H384">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="385" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A385" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B385">
+        <v>988.6</v>
+      </c>
+      <c r="C385">
+        <v>499.1</v>
+      </c>
+      <c r="D385">
+        <v>78.2</v>
+      </c>
+      <c r="E385">
+        <v>31.9</v>
+      </c>
+      <c r="F385">
+        <v>363.7</v>
+      </c>
+      <c r="H385">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="386" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A386" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B386">
+        <v>995.9</v>
+      </c>
+      <c r="C386">
+        <v>510.1</v>
+      </c>
+      <c r="D386">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="E386">
+        <v>31.1</v>
+      </c>
+      <c r="F386">
+        <v>358.9</v>
+      </c>
+      <c r="H386">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="387" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A387" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B387">
+        <v>1003.5</v>
+      </c>
+      <c r="C387">
+        <v>518.5</v>
+      </c>
+      <c r="D387">
+        <v>80.2</v>
+      </c>
+      <c r="E387">
+        <v>32.6</v>
+      </c>
+      <c r="F387">
+        <v>355.4</v>
+      </c>
+      <c r="H387">
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="388" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A388" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B388">
+        <v>1016.4</v>
+      </c>
+      <c r="C388">
+        <v>529.29999999999995</v>
+      </c>
+      <c r="D388">
+        <v>84</v>
+      </c>
+      <c r="E388">
+        <v>31.4</v>
+      </c>
+      <c r="F388">
+        <v>352.8</v>
+      </c>
+      <c r="H388">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="389" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A389" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B389">
+        <v>1036.3</v>
+      </c>
+      <c r="C389">
+        <v>554.20000000000005</v>
+      </c>
+      <c r="D389">
+        <v>89.8</v>
+      </c>
+      <c r="E389">
+        <v>31.5</v>
+      </c>
+      <c r="F389">
+        <v>342.3</v>
+      </c>
+      <c r="H389">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="390" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A390" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B390">
+        <v>1034.4000000000001</v>
+      </c>
+      <c r="C390">
+        <v>559.20000000000005</v>
+      </c>
+      <c r="D390">
+        <v>90.7</v>
+      </c>
+      <c r="E390">
+        <v>31.6</v>
+      </c>
+      <c r="F390">
+        <v>334.8</v>
+      </c>
+      <c r="H390">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="391" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A391" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B391">
+        <v>1045.5</v>
+      </c>
+      <c r="C391">
+        <v>580.79999999999995</v>
+      </c>
+      <c r="D391">
+        <v>90.6</v>
+      </c>
+      <c r="E391">
+        <v>33</v>
+      </c>
+      <c r="F391">
+        <v>324</v>
+      </c>
+      <c r="H391">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="392" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A392" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B392">
+        <v>1070.2</v>
+      </c>
+      <c r="C392">
+        <v>602.9</v>
+      </c>
+      <c r="D392">
+        <v>90.2</v>
+      </c>
+      <c r="E392">
+        <v>33.4</v>
+      </c>
+      <c r="F392">
+        <v>324.7</v>
+      </c>
+      <c r="H392">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="393" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A393" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B393">
+        <v>1090.4000000000001</v>
+      </c>
+      <c r="C393">
+        <v>610.9</v>
+      </c>
+      <c r="D393">
+        <v>92.7</v>
+      </c>
+      <c r="E393">
+        <v>39.1</v>
+      </c>
+      <c r="F393">
+        <v>331.7</v>
+      </c>
+      <c r="H393">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="394" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A394" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B394">
+        <v>1091.9000000000001</v>
+      </c>
+      <c r="C394">
+        <v>611.29999999999995</v>
+      </c>
+      <c r="D394">
+        <v>94</v>
+      </c>
+      <c r="E394">
+        <v>40.6</v>
+      </c>
+      <c r="F394">
+        <v>326.60000000000002</v>
+      </c>
+      <c r="H394">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="395" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A395" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B395">
+        <v>1102.0999999999999</v>
+      </c>
+      <c r="C395">
+        <v>616</v>
+      </c>
+      <c r="D395">
+        <v>94</v>
+      </c>
+      <c r="E395">
+        <v>41.6</v>
+      </c>
+      <c r="F395">
+        <v>332.5</v>
+      </c>
+      <c r="H395">
+        <v>17.899999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10552,13 +10907,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Y380"/>
+  <dimension ref="A1:Y394"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A343" workbookViewId="0">
-      <selection activeCell="N373" sqref="N373"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E371" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="N376" sqref="N376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -10568,73 +10929,73 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>346</v>
+        <v>358</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>351</v>
+        <v>363</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>352</v>
+        <v>364</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>353</v>
+        <v>365</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>354</v>
+        <v>366</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>366</v>
-      </c>
       <c r="X1" s="1" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
@@ -34079,6 +34440,907 @@
       </c>
       <c r="X380">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="381" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A381" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B381">
+        <v>485.2</v>
+      </c>
+      <c r="C381">
+        <v>162.19999999999999</v>
+      </c>
+      <c r="D381">
+        <v>39.1</v>
+      </c>
+      <c r="E381">
+        <v>0.5</v>
+      </c>
+      <c r="F381">
+        <v>0</v>
+      </c>
+      <c r="G381">
+        <v>23.7</v>
+      </c>
+      <c r="H381">
+        <v>5.4</v>
+      </c>
+      <c r="I381">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="J381">
+        <v>68.5</v>
+      </c>
+      <c r="K381">
+        <v>17.3</v>
+      </c>
+      <c r="L381">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="M381">
+        <v>11.2</v>
+      </c>
+      <c r="N381">
+        <v>12.3</v>
+      </c>
+      <c r="P381">
+        <v>2.4</v>
+      </c>
+      <c r="Q381">
+        <v>1.4</v>
+      </c>
+      <c r="T381">
+        <v>0</v>
+      </c>
+      <c r="U381">
+        <v>0.2</v>
+      </c>
+      <c r="V381">
+        <v>6</v>
+      </c>
+      <c r="W381">
+        <v>80.2</v>
+      </c>
+      <c r="X381">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="382" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A382" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B382">
+        <v>497.4</v>
+      </c>
+      <c r="C382">
+        <v>159.6</v>
+      </c>
+      <c r="D382">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="E382">
+        <v>0.9</v>
+      </c>
+      <c r="F382">
+        <v>0</v>
+      </c>
+      <c r="G382">
+        <v>24.5</v>
+      </c>
+      <c r="H382">
+        <v>5.6</v>
+      </c>
+      <c r="I382">
+        <v>36.9</v>
+      </c>
+      <c r="J382">
+        <v>69</v>
+      </c>
+      <c r="K382">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="L382">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="M382">
+        <v>11.3</v>
+      </c>
+      <c r="N382">
+        <v>12.6</v>
+      </c>
+      <c r="P382">
+        <v>2.4</v>
+      </c>
+      <c r="Q382">
+        <v>1.4</v>
+      </c>
+      <c r="T382">
+        <v>0.1</v>
+      </c>
+      <c r="U382">
+        <v>0.2</v>
+      </c>
+      <c r="V382">
+        <v>6.1</v>
+      </c>
+      <c r="W382">
+        <v>89.1</v>
+      </c>
+      <c r="X382">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="383" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A383" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B383">
+        <v>501.5</v>
+      </c>
+      <c r="C383">
+        <v>171.2</v>
+      </c>
+      <c r="D383">
+        <v>41.3</v>
+      </c>
+      <c r="E383">
+        <v>0.8</v>
+      </c>
+      <c r="F383">
+        <v>0</v>
+      </c>
+      <c r="G383">
+        <v>25.8</v>
+      </c>
+      <c r="H383">
+        <v>5.5</v>
+      </c>
+      <c r="I383">
+        <v>38.4</v>
+      </c>
+      <c r="J383">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="K383">
+        <v>19.5</v>
+      </c>
+      <c r="L383">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="M383">
+        <v>11.9</v>
+      </c>
+      <c r="N383">
+        <v>12.4</v>
+      </c>
+      <c r="P383">
+        <v>2.4</v>
+      </c>
+      <c r="Q383">
+        <v>1.4</v>
+      </c>
+      <c r="T383">
+        <v>0.1</v>
+      </c>
+      <c r="U383">
+        <v>0.2</v>
+      </c>
+      <c r="V383">
+        <v>5.8</v>
+      </c>
+      <c r="W383">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="X383">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="384" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A384" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B384">
+        <v>499.1</v>
+      </c>
+      <c r="C384">
+        <v>171.6</v>
+      </c>
+      <c r="D384">
+        <v>40.9</v>
+      </c>
+      <c r="E384">
+        <v>0.4</v>
+      </c>
+      <c r="F384">
+        <v>0</v>
+      </c>
+      <c r="G384">
+        <v>26.5</v>
+      </c>
+      <c r="H384">
+        <v>6.4</v>
+      </c>
+      <c r="I384">
+        <v>38.1</v>
+      </c>
+      <c r="J384">
+        <v>69.8</v>
+      </c>
+      <c r="K384">
+        <v>19.3</v>
+      </c>
+      <c r="L384">
+        <v>16.8</v>
+      </c>
+      <c r="M384">
+        <v>12</v>
+      </c>
+      <c r="N384">
+        <v>12.1</v>
+      </c>
+      <c r="P384">
+        <v>2.5</v>
+      </c>
+      <c r="Q384">
+        <v>1.4</v>
+      </c>
+      <c r="T384">
+        <v>0.1</v>
+      </c>
+      <c r="U384">
+        <v>0.2</v>
+      </c>
+      <c r="V384">
+        <v>5.8</v>
+      </c>
+      <c r="W384">
+        <v>74.7</v>
+      </c>
+      <c r="X384">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="385" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A385" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B385">
+        <v>510.1</v>
+      </c>
+      <c r="C385">
+        <v>179.1</v>
+      </c>
+      <c r="D385">
+        <v>42</v>
+      </c>
+      <c r="E385">
+        <v>0.5</v>
+      </c>
+      <c r="F385">
+        <v>0</v>
+      </c>
+      <c r="G385">
+        <v>26.7</v>
+      </c>
+      <c r="H385">
+        <v>7.2</v>
+      </c>
+      <c r="I385">
+        <v>38.5</v>
+      </c>
+      <c r="J385">
+        <v>70.7</v>
+      </c>
+      <c r="K385">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="L385">
+        <v>16.8</v>
+      </c>
+      <c r="M385">
+        <v>12.5</v>
+      </c>
+      <c r="N385">
+        <v>12.1</v>
+      </c>
+      <c r="P385">
+        <v>2.4</v>
+      </c>
+      <c r="Q385">
+        <v>1.4</v>
+      </c>
+      <c r="T385">
+        <v>0.1</v>
+      </c>
+      <c r="U385">
+        <v>0.2</v>
+      </c>
+      <c r="V385">
+        <v>6.2</v>
+      </c>
+      <c r="W385">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="X385">
+        <v>0.6</v>
+      </c>
+      <c r="Y385">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A386" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B386">
+        <v>518.5</v>
+      </c>
+      <c r="C386">
+        <v>181.7</v>
+      </c>
+      <c r="D386">
+        <v>42.8</v>
+      </c>
+      <c r="E386">
+        <v>0.6</v>
+      </c>
+      <c r="F386">
+        <v>0</v>
+      </c>
+      <c r="G386">
+        <v>27</v>
+      </c>
+      <c r="H386">
+        <v>6.5</v>
+      </c>
+      <c r="I386">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="J386">
+        <v>76.2</v>
+      </c>
+      <c r="K386">
+        <v>18.3</v>
+      </c>
+      <c r="L386">
+        <v>16.7</v>
+      </c>
+      <c r="M386">
+        <v>12</v>
+      </c>
+      <c r="N386">
+        <v>12.1</v>
+      </c>
+      <c r="P386">
+        <v>2.5</v>
+      </c>
+      <c r="Q386">
+        <v>1.4</v>
+      </c>
+      <c r="T386">
+        <v>0.1</v>
+      </c>
+      <c r="U386">
+        <v>0.2</v>
+      </c>
+      <c r="V386">
+        <v>7</v>
+      </c>
+      <c r="W386">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="X386">
+        <v>0.7</v>
+      </c>
+      <c r="Y386">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="387" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A387" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B387">
+        <v>529.29999999999995</v>
+      </c>
+      <c r="C387">
+        <v>192</v>
+      </c>
+      <c r="D387">
+        <v>42.6</v>
+      </c>
+      <c r="E387">
+        <v>0.7</v>
+      </c>
+      <c r="F387">
+        <v>0</v>
+      </c>
+      <c r="G387">
+        <v>27.5</v>
+      </c>
+      <c r="H387">
+        <v>6.9</v>
+      </c>
+      <c r="I387">
+        <v>40</v>
+      </c>
+      <c r="J387">
+        <v>75.5</v>
+      </c>
+      <c r="K387">
+        <v>18.5</v>
+      </c>
+      <c r="L387">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="M387">
+        <v>12</v>
+      </c>
+      <c r="N387">
+        <v>12</v>
+      </c>
+      <c r="P387">
+        <v>2.6</v>
+      </c>
+      <c r="Q387">
+        <v>1.4</v>
+      </c>
+      <c r="T387">
+        <v>0.1</v>
+      </c>
+      <c r="U387">
+        <v>0.2</v>
+      </c>
+      <c r="V387">
+        <v>7</v>
+      </c>
+      <c r="W387">
+        <v>73.7</v>
+      </c>
+      <c r="X387">
+        <v>0.6</v>
+      </c>
+      <c r="Y387">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="388" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A388" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B388">
+        <v>554.20000000000005</v>
+      </c>
+      <c r="C388">
+        <v>206.6</v>
+      </c>
+      <c r="D388">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="E388">
+        <v>0.2</v>
+      </c>
+      <c r="G388">
+        <v>27.1</v>
+      </c>
+      <c r="H388">
+        <v>5.4</v>
+      </c>
+      <c r="I388">
+        <v>40</v>
+      </c>
+      <c r="J388">
+        <v>76.3</v>
+      </c>
+      <c r="K388">
+        <v>21.4</v>
+      </c>
+      <c r="L388">
+        <v>16.7</v>
+      </c>
+      <c r="M388">
+        <v>12.2</v>
+      </c>
+      <c r="N388">
+        <v>11.9</v>
+      </c>
+      <c r="P388">
+        <v>2.5</v>
+      </c>
+      <c r="Q388">
+        <v>1.4</v>
+      </c>
+      <c r="T388">
+        <v>0.1</v>
+      </c>
+      <c r="U388">
+        <v>0.2</v>
+      </c>
+      <c r="V388">
+        <v>7.6</v>
+      </c>
+      <c r="W388">
+        <v>83.3</v>
+      </c>
+      <c r="X388">
+        <v>0.6</v>
+      </c>
+      <c r="Y388">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A389" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B389">
+        <v>559.20000000000005</v>
+      </c>
+      <c r="C389">
+        <v>208</v>
+      </c>
+      <c r="D389">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="E389">
+        <v>0.3</v>
+      </c>
+      <c r="G389">
+        <v>29.3</v>
+      </c>
+      <c r="H389">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I389">
+        <v>41.3</v>
+      </c>
+      <c r="J389">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="K389">
+        <v>21.1</v>
+      </c>
+      <c r="L389">
+        <v>15.9</v>
+      </c>
+      <c r="M389">
+        <v>13.2</v>
+      </c>
+      <c r="N389">
+        <v>12.2</v>
+      </c>
+      <c r="P389">
+        <v>2.5</v>
+      </c>
+      <c r="Q389">
+        <v>1.4</v>
+      </c>
+      <c r="T389">
+        <v>0.1</v>
+      </c>
+      <c r="U389">
+        <v>0.2</v>
+      </c>
+      <c r="V389">
+        <v>7.5</v>
+      </c>
+      <c r="W389">
+        <v>83.2</v>
+      </c>
+      <c r="X389">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="390" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A390" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B390">
+        <v>580.79999999999995</v>
+      </c>
+      <c r="C390">
+        <v>212.9</v>
+      </c>
+      <c r="D390">
+        <v>41.9</v>
+      </c>
+      <c r="E390">
+        <v>1.4</v>
+      </c>
+      <c r="G390">
+        <v>31.1</v>
+      </c>
+      <c r="H390">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I390">
+        <v>43.9</v>
+      </c>
+      <c r="J390">
+        <v>84.7</v>
+      </c>
+      <c r="K390">
+        <v>23</v>
+      </c>
+      <c r="L390">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="M390">
+        <v>14.4</v>
+      </c>
+      <c r="N390">
+        <v>12.1</v>
+      </c>
+      <c r="P390">
+        <v>2.5</v>
+      </c>
+      <c r="Q390">
+        <v>1.4</v>
+      </c>
+      <c r="T390">
+        <v>0.1</v>
+      </c>
+      <c r="U390">
+        <v>0.2</v>
+      </c>
+      <c r="V390">
+        <v>7.2</v>
+      </c>
+      <c r="W390">
+        <v>82.6</v>
+      </c>
+      <c r="X390">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="391" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A391" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B391">
+        <v>602.9</v>
+      </c>
+      <c r="C391">
+        <v>230.7</v>
+      </c>
+      <c r="D391">
+        <v>43.7</v>
+      </c>
+      <c r="E391">
+        <v>1.7</v>
+      </c>
+      <c r="G391">
+        <v>31.7</v>
+      </c>
+      <c r="H391">
+        <v>5.3</v>
+      </c>
+      <c r="I391">
+        <v>43.8</v>
+      </c>
+      <c r="J391">
+        <v>85.5</v>
+      </c>
+      <c r="K391">
+        <v>22.9</v>
+      </c>
+      <c r="L391">
+        <v>16.3</v>
+      </c>
+      <c r="M391">
+        <v>14.7</v>
+      </c>
+      <c r="N391">
+        <v>12.7</v>
+      </c>
+      <c r="P391">
+        <v>2.6</v>
+      </c>
+      <c r="Q391">
+        <v>1.4</v>
+      </c>
+      <c r="T391">
+        <v>0.1</v>
+      </c>
+      <c r="U391">
+        <v>0.1</v>
+      </c>
+      <c r="V391">
+        <v>7.1</v>
+      </c>
+      <c r="W391">
+        <v>82</v>
+      </c>
+      <c r="X391">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="392" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A392" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B392">
+        <v>610.9</v>
+      </c>
+      <c r="C392">
+        <v>235.4</v>
+      </c>
+      <c r="D392">
+        <v>45.1</v>
+      </c>
+      <c r="E392">
+        <v>1.2</v>
+      </c>
+      <c r="G392">
+        <v>31.5</v>
+      </c>
+      <c r="H392">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I392">
+        <v>43.3</v>
+      </c>
+      <c r="J392">
+        <v>90</v>
+      </c>
+      <c r="K392">
+        <v>22</v>
+      </c>
+      <c r="L392">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="M392">
+        <v>15</v>
+      </c>
+      <c r="N392">
+        <v>12.9</v>
+      </c>
+      <c r="P392">
+        <v>2.6</v>
+      </c>
+      <c r="Q392">
+        <v>1.4</v>
+      </c>
+      <c r="T392">
+        <v>0.1</v>
+      </c>
+      <c r="U392">
+        <v>0.1</v>
+      </c>
+      <c r="V392">
+        <v>7.5</v>
+      </c>
+      <c r="W392">
+        <v>81.099999999999994</v>
+      </c>
+      <c r="X392">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="393" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A393" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B393">
+        <v>611.29999999999995</v>
+      </c>
+      <c r="C393">
+        <v>235.6</v>
+      </c>
+      <c r="D393">
+        <v>45.6</v>
+      </c>
+      <c r="E393">
+        <v>1</v>
+      </c>
+      <c r="G393">
+        <v>30.6</v>
+      </c>
+      <c r="H393">
+        <v>5.6</v>
+      </c>
+      <c r="I393">
+        <v>43.8</v>
+      </c>
+      <c r="J393">
+        <v>94.2</v>
+      </c>
+      <c r="K393">
+        <v>23</v>
+      </c>
+      <c r="L393">
+        <v>14.2</v>
+      </c>
+      <c r="M393">
+        <v>15.1</v>
+      </c>
+      <c r="N393">
+        <v>12.1</v>
+      </c>
+      <c r="P393">
+        <v>2.6</v>
+      </c>
+      <c r="Q393">
+        <v>1.4</v>
+      </c>
+      <c r="T393">
+        <v>0.1</v>
+      </c>
+      <c r="U393">
+        <v>0.1</v>
+      </c>
+      <c r="V393">
+        <v>6.8</v>
+      </c>
+      <c r="W393">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="X393">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="394" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A394" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B394">
+        <v>616</v>
+      </c>
+      <c r="C394">
+        <v>234.9</v>
+      </c>
+      <c r="D394">
+        <v>48.3</v>
+      </c>
+      <c r="E394">
+        <v>1.3</v>
+      </c>
+      <c r="G394">
+        <v>32.1</v>
+      </c>
+      <c r="H394">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="I394">
+        <v>45.3</v>
+      </c>
+      <c r="J394">
+        <v>92.5</v>
+      </c>
+      <c r="K394">
+        <v>25.1</v>
+      </c>
+      <c r="L394">
+        <v>13.8</v>
+      </c>
+      <c r="M394">
+        <v>15</v>
+      </c>
+      <c r="N394">
+        <v>12.2</v>
+      </c>
+      <c r="P394">
+        <v>2.6</v>
+      </c>
+      <c r="Q394">
+        <v>1.4</v>
+      </c>
+      <c r="T394">
+        <v>0.1</v>
+      </c>
+      <c r="U394">
+        <v>0.1</v>
+      </c>
+      <c r="V394">
+        <v>6.8</v>
+      </c>
+      <c r="W394">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="X394">
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>
@@ -34088,7 +35350,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J376"/>
+  <dimension ref="A1:J390"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -34102,28 +35364,28 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>356</v>
+        <v>367</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>354</v>
+        <v>366</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>362</v>
+        <v>373</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>369</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -37059,7 +38321,7 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>370</v>
+        <v>382</v>
       </c>
       <c r="B113">
         <v>47.4</v>
@@ -44041,6 +45303,367 @@
         <v>32</v>
       </c>
       <c r="I376">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="377" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A377" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B377">
+        <v>74.8</v>
+      </c>
+      <c r="C377">
+        <v>14.7</v>
+      </c>
+      <c r="D377">
+        <v>5</v>
+      </c>
+      <c r="E377">
+        <v>21.3</v>
+      </c>
+      <c r="G377">
+        <v>1.2</v>
+      </c>
+      <c r="H377">
+        <v>32.700000000000003</v>
+      </c>
+    </row>
+    <row r="378" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A378" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B378">
+        <v>75.8</v>
+      </c>
+      <c r="C378">
+        <v>14.5</v>
+      </c>
+      <c r="D378">
+        <v>5</v>
+      </c>
+      <c r="E378">
+        <v>22.3</v>
+      </c>
+      <c r="G378">
+        <v>1.4</v>
+      </c>
+      <c r="H378">
+        <v>32.6</v>
+      </c>
+      <c r="I378">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="379" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A379" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B379">
+        <v>78</v>
+      </c>
+      <c r="C379">
+        <v>16</v>
+      </c>
+      <c r="D379">
+        <v>5.2</v>
+      </c>
+      <c r="E379">
+        <v>22.6</v>
+      </c>
+      <c r="G379">
+        <v>1.5</v>
+      </c>
+      <c r="H379">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="I379">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="380" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A380" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B380">
+        <v>78.2</v>
+      </c>
+      <c r="C380">
+        <v>16.3</v>
+      </c>
+      <c r="D380">
+        <v>5.2</v>
+      </c>
+      <c r="E380">
+        <v>22.2</v>
+      </c>
+      <c r="G380">
+        <v>1.4</v>
+      </c>
+      <c r="H380">
+        <v>33.1</v>
+      </c>
+      <c r="I380">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="381" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A381" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B381">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="C381">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="D381">
+        <v>5.4</v>
+      </c>
+      <c r="E381">
+        <v>23.2</v>
+      </c>
+      <c r="G381">
+        <v>1.6</v>
+      </c>
+      <c r="H381">
+        <v>31.8</v>
+      </c>
+      <c r="I381">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="382" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A382" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B382">
+        <v>80.2</v>
+      </c>
+      <c r="C382">
+        <v>18.7</v>
+      </c>
+      <c r="D382">
+        <v>5.4</v>
+      </c>
+      <c r="E382">
+        <v>23.4</v>
+      </c>
+      <c r="G382">
+        <v>1.6</v>
+      </c>
+      <c r="H382">
+        <v>31.1</v>
+      </c>
+      <c r="I382">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="383" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A383" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B383">
+        <v>84</v>
+      </c>
+      <c r="C383">
+        <v>20</v>
+      </c>
+      <c r="D383">
+        <v>5.5</v>
+      </c>
+      <c r="E383">
+        <v>23.7</v>
+      </c>
+      <c r="G383">
+        <v>1.7</v>
+      </c>
+      <c r="H383">
+        <v>33</v>
+      </c>
+      <c r="I383">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="384" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A384" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B384">
+        <v>89.8</v>
+      </c>
+      <c r="C384">
+        <v>20.6</v>
+      </c>
+      <c r="D384">
+        <v>5.7</v>
+      </c>
+      <c r="E384">
+        <v>24.2</v>
+      </c>
+      <c r="G384">
+        <v>1.8</v>
+      </c>
+      <c r="H384">
+        <v>37.5</v>
+      </c>
+      <c r="I384">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="385" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A385" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B385">
+        <v>90.7</v>
+      </c>
+      <c r="C385">
+        <v>21.3</v>
+      </c>
+      <c r="D385">
+        <v>5.5</v>
+      </c>
+      <c r="E385">
+        <v>23.9</v>
+      </c>
+      <c r="G385">
+        <v>1.7</v>
+      </c>
+      <c r="H385">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="I385">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A386" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B386">
+        <v>90.6</v>
+      </c>
+      <c r="C386">
+        <v>21.1</v>
+      </c>
+      <c r="D386">
+        <v>5.4</v>
+      </c>
+      <c r="E386">
+        <v>24.3</v>
+      </c>
+      <c r="G386">
+        <v>1.8</v>
+      </c>
+      <c r="H386">
+        <v>38</v>
+      </c>
+      <c r="I386">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="387" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A387" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B387">
+        <v>90.2</v>
+      </c>
+      <c r="C387">
+        <v>22</v>
+      </c>
+      <c r="D387">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E387">
+        <v>23.8</v>
+      </c>
+      <c r="G387">
+        <v>1.9</v>
+      </c>
+      <c r="H387">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="I387">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="388" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A388" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B388">
+        <v>92.7</v>
+      </c>
+      <c r="C388">
+        <v>23.1</v>
+      </c>
+      <c r="D388">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E388">
+        <v>23.9</v>
+      </c>
+      <c r="G388">
+        <v>1.9</v>
+      </c>
+      <c r="H388">
+        <v>38.6</v>
+      </c>
+      <c r="I388">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A389" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B389">
+        <v>94</v>
+      </c>
+      <c r="C389">
+        <v>24.4</v>
+      </c>
+      <c r="D389">
+        <v>6.3</v>
+      </c>
+      <c r="E389">
+        <v>23.8</v>
+      </c>
+      <c r="G389">
+        <v>1.9</v>
+      </c>
+      <c r="H389">
+        <v>37.6</v>
+      </c>
+      <c r="I389">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="390" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A390" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B390">
+        <v>94</v>
+      </c>
+      <c r="C390">
+        <v>24.9</v>
+      </c>
+      <c r="D390">
+        <v>6.5</v>
+      </c>
+      <c r="E390">
+        <v>23.2</v>
+      </c>
+      <c r="G390">
+        <v>1.7</v>
+      </c>
+      <c r="H390">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="I390">
         <v>0</v>
       </c>
     </row>
@@ -44051,7 +45674,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K378"/>
+  <dimension ref="A1:K392"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -44065,31 +45688,31 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>352</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>365</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -46827,7 +48450,7 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>370</v>
+        <v>382</v>
       </c>
       <c r="B113">
         <v>33.4</v>
@@ -53115,6 +54738,328 @@
       </c>
       <c r="H378">
         <v>0</v>
+      </c>
+    </row>
+    <row r="379" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A379" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B379">
+        <v>34.1</v>
+      </c>
+      <c r="C379">
+        <v>17.3</v>
+      </c>
+      <c r="D379">
+        <v>10.8</v>
+      </c>
+      <c r="E379">
+        <v>2.7</v>
+      </c>
+      <c r="F379">
+        <v>3.2</v>
+      </c>
+      <c r="H379">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="380" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A380" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B380">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="C380">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="D380">
+        <v>10.6</v>
+      </c>
+      <c r="E380">
+        <v>3.2</v>
+      </c>
+      <c r="F380">
+        <v>3.4</v>
+      </c>
+      <c r="H380">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="381" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A381" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B381">
+        <v>33.9</v>
+      </c>
+      <c r="C381">
+        <v>17.5</v>
+      </c>
+      <c r="D381">
+        <v>9.6</v>
+      </c>
+      <c r="E381">
+        <v>3.2</v>
+      </c>
+      <c r="F381">
+        <v>3.6</v>
+      </c>
+      <c r="H381">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="382" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A382" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B382">
+        <v>31.9</v>
+      </c>
+      <c r="C382">
+        <v>17.7</v>
+      </c>
+      <c r="D382">
+        <v>9.1</v>
+      </c>
+      <c r="E382">
+        <v>1.7</v>
+      </c>
+      <c r="F382">
+        <v>3.5</v>
+      </c>
+      <c r="H382">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="383" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A383" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B383">
+        <v>31.1</v>
+      </c>
+      <c r="C383">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="D383">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E383">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F383">
+        <v>3.4</v>
+      </c>
+      <c r="H383">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="384" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A384" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B384">
+        <v>32.6</v>
+      </c>
+      <c r="C384">
+        <v>17.7</v>
+      </c>
+      <c r="D384">
+        <v>8.4</v>
+      </c>
+      <c r="E384">
+        <v>3</v>
+      </c>
+      <c r="F384">
+        <v>3.4</v>
+      </c>
+      <c r="H384">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="385" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A385" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B385">
+        <v>31.4</v>
+      </c>
+      <c r="C385">
+        <v>18</v>
+      </c>
+      <c r="D385">
+        <v>8.1</v>
+      </c>
+      <c r="E385">
+        <v>1.6</v>
+      </c>
+      <c r="F385">
+        <v>3.7</v>
+      </c>
+      <c r="H385">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A386" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B386">
+        <v>31.5</v>
+      </c>
+      <c r="C386">
+        <v>18.7</v>
+      </c>
+      <c r="D386">
+        <v>7.3</v>
+      </c>
+      <c r="E386">
+        <v>1.6</v>
+      </c>
+      <c r="F386">
+        <v>3.8</v>
+      </c>
+      <c r="H386">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="387" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A387" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B387">
+        <v>31.6</v>
+      </c>
+      <c r="C387">
+        <v>18.8</v>
+      </c>
+      <c r="D387">
+        <v>7.5</v>
+      </c>
+      <c r="E387">
+        <v>1.6</v>
+      </c>
+      <c r="F387">
+        <v>3.8</v>
+      </c>
+      <c r="H387">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="388" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A388" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B388">
+        <v>33</v>
+      </c>
+      <c r="C388">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="D388">
+        <v>8</v>
+      </c>
+      <c r="E388">
+        <v>1.7</v>
+      </c>
+      <c r="F388">
+        <v>4</v>
+      </c>
+      <c r="H388">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="389" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A389" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B389">
+        <v>33.4</v>
+      </c>
+      <c r="C389">
+        <v>19.2</v>
+      </c>
+      <c r="D389">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E389">
+        <v>1.5</v>
+      </c>
+      <c r="F389">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H389">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="390" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A390" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B390">
+        <v>39.1</v>
+      </c>
+      <c r="C390">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="D390">
+        <v>11.9</v>
+      </c>
+      <c r="E390">
+        <v>1.9</v>
+      </c>
+      <c r="F390">
+        <v>5</v>
+      </c>
+      <c r="H390">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="391" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A391" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B391">
+        <v>40.6</v>
+      </c>
+      <c r="C391">
+        <v>20.9</v>
+      </c>
+      <c r="D391">
+        <v>11.7</v>
+      </c>
+      <c r="E391">
+        <v>3.1</v>
+      </c>
+      <c r="F391">
+        <v>4.7</v>
+      </c>
+      <c r="H391">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="392" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A392" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B392">
+        <v>41.6</v>
+      </c>
+      <c r="C392">
+        <v>21.5</v>
+      </c>
+      <c r="D392">
+        <v>12.2</v>
+      </c>
+      <c r="E392">
+        <v>3.3</v>
+      </c>
+      <c r="F392">
+        <v>4.5</v>
+      </c>
+      <c r="H392">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -53124,7 +55069,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:M381"/>
+  <dimension ref="A1:M395"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -53138,37 +55083,37 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>369</v>
+        <v>381</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>373</v>
+        <v>385</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>356</v>
+        <v>367</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>360</v>
+        <v>371</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>352</v>
+        <v>364</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>374</v>
+        <v>386</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>346</v>
+        <v>358</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>375</v>
+        <v>387</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>355</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -65524,6 +67469,496 @@
       </c>
       <c r="M381">
         <v>74.400000000000006</v>
+      </c>
+    </row>
+    <row r="382" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A382" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B382">
+        <v>369.3</v>
+      </c>
+      <c r="C382">
+        <v>87.9</v>
+      </c>
+      <c r="D382">
+        <v>54.4</v>
+      </c>
+      <c r="E382">
+        <v>102.1</v>
+      </c>
+      <c r="G382">
+        <v>11.5</v>
+      </c>
+      <c r="H382">
+        <v>14.8</v>
+      </c>
+      <c r="I382">
+        <v>17.7</v>
+      </c>
+      <c r="J382">
+        <v>6.6</v>
+      </c>
+      <c r="L382">
+        <v>0</v>
+      </c>
+      <c r="M382">
+        <v>74.3</v>
+      </c>
+    </row>
+    <row r="383" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A383" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B383">
+        <v>368.8</v>
+      </c>
+      <c r="C383">
+        <v>89.3</v>
+      </c>
+      <c r="D383">
+        <v>55.5</v>
+      </c>
+      <c r="E383">
+        <v>101.9</v>
+      </c>
+      <c r="G383">
+        <v>11.3</v>
+      </c>
+      <c r="H383">
+        <v>14.7</v>
+      </c>
+      <c r="I383">
+        <v>18</v>
+      </c>
+      <c r="J383">
+        <v>6.3</v>
+      </c>
+      <c r="L383">
+        <v>0</v>
+      </c>
+      <c r="M383">
+        <v>71.599999999999994</v>
+      </c>
+    </row>
+    <row r="384" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A384" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B384">
+        <v>365.1</v>
+      </c>
+      <c r="C384">
+        <v>91.6</v>
+      </c>
+      <c r="D384">
+        <v>47.5</v>
+      </c>
+      <c r="E384">
+        <v>105.7</v>
+      </c>
+      <c r="G384">
+        <v>11.6</v>
+      </c>
+      <c r="H384">
+        <v>14.5</v>
+      </c>
+      <c r="I384">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="J384">
+        <v>6.2</v>
+      </c>
+      <c r="L384">
+        <v>0</v>
+      </c>
+      <c r="M384">
+        <v>69.599999999999994</v>
+      </c>
+    </row>
+    <row r="385" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A385" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B385">
+        <v>363.7</v>
+      </c>
+      <c r="C385">
+        <v>92</v>
+      </c>
+      <c r="D385">
+        <v>46.2</v>
+      </c>
+      <c r="E385">
+        <v>104.6</v>
+      </c>
+      <c r="G385">
+        <v>11.8</v>
+      </c>
+      <c r="H385">
+        <v>14.3</v>
+      </c>
+      <c r="I385">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="J385">
+        <v>6.1</v>
+      </c>
+      <c r="L385">
+        <v>0</v>
+      </c>
+      <c r="M385">
+        <v>69.8</v>
+      </c>
+    </row>
+    <row r="386" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A386" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B386">
+        <v>358.9</v>
+      </c>
+      <c r="C386">
+        <v>90.3</v>
+      </c>
+      <c r="D386">
+        <v>45.1</v>
+      </c>
+      <c r="E386">
+        <v>104.3</v>
+      </c>
+      <c r="G386">
+        <v>11.7</v>
+      </c>
+      <c r="H386">
+        <v>14.1</v>
+      </c>
+      <c r="I386">
+        <v>18.7</v>
+      </c>
+      <c r="J386">
+        <v>5.8</v>
+      </c>
+      <c r="L386">
+        <v>0</v>
+      </c>
+      <c r="M386">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="387" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A387" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B387">
+        <v>355.4</v>
+      </c>
+      <c r="C387">
+        <v>92</v>
+      </c>
+      <c r="D387">
+        <v>44.2</v>
+      </c>
+      <c r="E387">
+        <v>102.3</v>
+      </c>
+      <c r="G387">
+        <v>12</v>
+      </c>
+      <c r="H387">
+        <v>13.8</v>
+      </c>
+      <c r="I387">
+        <v>18.7</v>
+      </c>
+      <c r="J387">
+        <v>5.7</v>
+      </c>
+      <c r="L387">
+        <v>0</v>
+      </c>
+      <c r="M387">
+        <v>66.7</v>
+      </c>
+    </row>
+    <row r="388" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A388" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B388">
+        <v>352.8</v>
+      </c>
+      <c r="C388">
+        <v>92.2</v>
+      </c>
+      <c r="D388">
+        <v>43.6</v>
+      </c>
+      <c r="E388">
+        <v>101</v>
+      </c>
+      <c r="G388">
+        <v>11.8</v>
+      </c>
+      <c r="H388">
+        <v>13.3</v>
+      </c>
+      <c r="I388">
+        <v>18.8</v>
+      </c>
+      <c r="J388">
+        <v>5.6</v>
+      </c>
+      <c r="L388">
+        <v>0</v>
+      </c>
+      <c r="M388">
+        <v>66.5</v>
+      </c>
+    </row>
+    <row r="389" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A389" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B389">
+        <v>342.3</v>
+      </c>
+      <c r="C389">
+        <v>93</v>
+      </c>
+      <c r="D389">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="E389">
+        <v>99.8</v>
+      </c>
+      <c r="G389">
+        <v>11.5</v>
+      </c>
+      <c r="H389">
+        <v>12.6</v>
+      </c>
+      <c r="I389">
+        <v>19.3</v>
+      </c>
+      <c r="J389">
+        <v>5.3</v>
+      </c>
+      <c r="L389">
+        <v>0</v>
+      </c>
+      <c r="M389">
+        <v>61.2</v>
+      </c>
+    </row>
+    <row r="390" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A390" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B390">
+        <v>334.8</v>
+      </c>
+      <c r="C390">
+        <v>94.5</v>
+      </c>
+      <c r="D390">
+        <v>41.6</v>
+      </c>
+      <c r="E390">
+        <v>99.1</v>
+      </c>
+      <c r="G390">
+        <v>11.4</v>
+      </c>
+      <c r="H390">
+        <v>12.8</v>
+      </c>
+      <c r="I390">
+        <v>19.5</v>
+      </c>
+      <c r="J390">
+        <v>5.2</v>
+      </c>
+      <c r="L390">
+        <v>0</v>
+      </c>
+      <c r="M390">
+        <v>50.9</v>
+      </c>
+    </row>
+    <row r="391" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A391" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B391">
+        <v>324</v>
+      </c>
+      <c r="C391">
+        <v>94.8</v>
+      </c>
+      <c r="D391">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="E391">
+        <v>98.7</v>
+      </c>
+      <c r="G391">
+        <v>10.8</v>
+      </c>
+      <c r="H391">
+        <v>12.7</v>
+      </c>
+      <c r="I391">
+        <v>19.5</v>
+      </c>
+      <c r="J391">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="L391">
+        <v>0</v>
+      </c>
+      <c r="M391">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="392" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A392" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B392">
+        <v>324.7</v>
+      </c>
+      <c r="C392">
+        <v>95.8</v>
+      </c>
+      <c r="D392">
+        <v>41.1</v>
+      </c>
+      <c r="E392">
+        <v>98.1</v>
+      </c>
+      <c r="G392">
+        <v>11.2</v>
+      </c>
+      <c r="H392">
+        <v>13.8</v>
+      </c>
+      <c r="I392">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="J392">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L392">
+        <v>0</v>
+      </c>
+      <c r="M392">
+        <v>40.9</v>
+      </c>
+    </row>
+    <row r="393" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A393" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B393">
+        <v>331.7</v>
+      </c>
+      <c r="C393">
+        <v>98.8</v>
+      </c>
+      <c r="D393">
+        <v>45.1</v>
+      </c>
+      <c r="E393">
+        <v>96.5</v>
+      </c>
+      <c r="G393">
+        <v>11.5</v>
+      </c>
+      <c r="H393">
+        <v>14</v>
+      </c>
+      <c r="I393">
+        <v>19.5</v>
+      </c>
+      <c r="J393">
+        <v>4.7</v>
+      </c>
+      <c r="L393">
+        <v>0</v>
+      </c>
+      <c r="M393">
+        <v>41.6</v>
+      </c>
+    </row>
+    <row r="394" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A394" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B394">
+        <v>326.60000000000002</v>
+      </c>
+      <c r="C394">
+        <v>97.1</v>
+      </c>
+      <c r="D394">
+        <v>44</v>
+      </c>
+      <c r="E394">
+        <v>93.6</v>
+      </c>
+      <c r="G394">
+        <v>11.5</v>
+      </c>
+      <c r="H394">
+        <v>13.8</v>
+      </c>
+      <c r="I394">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="J394">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="L394">
+        <v>0</v>
+      </c>
+      <c r="M394">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="395" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A395" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B395">
+        <v>332.5</v>
+      </c>
+      <c r="C395">
+        <v>98.8</v>
+      </c>
+      <c r="D395">
+        <v>43.6</v>
+      </c>
+      <c r="E395">
+        <v>93.5</v>
+      </c>
+      <c r="G395">
+        <v>11.5</v>
+      </c>
+      <c r="H395">
+        <v>15</v>
+      </c>
+      <c r="I395">
+        <v>20</v>
+      </c>
+      <c r="J395">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="L395">
+        <v>0</v>
+      </c>
+      <c r="M395">
+        <v>45.2</v>
       </c>
     </row>
   </sheetData>
@@ -65533,7 +67968,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C117"/>
+  <dimension ref="A1:C131"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -65547,7 +67982,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>376</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -66824,6 +69259,160 @@
       </c>
       <c r="C117">
         <v>16.5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B118">
+        <v>16.2</v>
+      </c>
+      <c r="C118">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B119">
+        <v>17.2</v>
+      </c>
+      <c r="C119">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B120">
+        <v>15.9</v>
+      </c>
+      <c r="C120">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B121">
+        <v>15.8</v>
+      </c>
+      <c r="C121">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B122">
+        <v>15.1</v>
+      </c>
+      <c r="C122">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B123">
+        <v>16.8</v>
+      </c>
+      <c r="C123">
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B124">
+        <v>19</v>
+      </c>
+      <c r="C124">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B125">
+        <v>18.5</v>
+      </c>
+      <c r="C125">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B126">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="C126">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B127">
+        <v>17.3</v>
+      </c>
+      <c r="C127">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B128">
+        <v>19</v>
+      </c>
+      <c r="C128">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B129">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="C129">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B130">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="C130">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B131">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="C131">
+        <v>17.899999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>